<commit_message>
updates: remove warnings, update feature list
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C232F300-6B14-46F5-94BE-3E7808AFA5F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430"/>
+    <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20180611" sheetId="8" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="60">
   <si>
     <t>State</t>
   </si>
@@ -193,13 +194,19 @@
   </si>
   <si>
     <t>not possible in CortexM family</t>
+  </si>
+  <si>
+    <t>see en.DM00046982.pdf page 192</t>
+  </si>
+  <si>
+    <t>on_hold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,13 +284,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -321,9 +336,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,9 +370,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,9 +422,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -564,20 +615,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="A38:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="4"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -605,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -616,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -630,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -641,7 +692,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -652,7 +703,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -663,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -674,7 +725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -685,7 +736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -696,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -707,7 +758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -718,7 +769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -732,9 +783,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>14</v>
@@ -742,8 +793,11 @@
       <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -754,10 +808,10 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -768,29 +822,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>13</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>13</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -801,7 +855,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -812,7 +866,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -823,7 +877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -834,18 +888,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -856,7 +910,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -867,7 +921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -878,7 +932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -889,7 +943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -900,7 +954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -911,7 +965,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -922,7 +976,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
@@ -933,12 +987,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -949,7 +1003,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -960,7 +1014,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -971,7 +1025,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
@@ -982,7 +1036,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -993,18 +1047,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>13</v>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>1</v>
       </c>
@@ -1022,20 +1076,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="4"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1063,7 +1117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1099,7 +1153,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1121,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1132,7 +1186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +1197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1219,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1230,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1187,7 +1241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1198,7 +1252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1212,7 +1266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1223,7 +1277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1237,7 +1291,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1248,7 +1302,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -1259,7 +1313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1281,7 +1335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +1346,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -1303,7 +1357,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1314,7 +1368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1379,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1336,7 +1390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1347,7 +1401,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1412,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1369,7 +1423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1380,7 +1434,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -1391,7 +1445,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
@@ -1402,7 +1456,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>1</v>
       </c>
@@ -1413,12 +1467,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1429,7 +1483,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1440,7 +1494,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1505,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -1462,7 +1516,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1473,7 +1527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>1</v>
       </c>
@@ -1484,7 +1538,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
@@ -1502,20 +1556,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="4"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1543,7 +1597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1554,7 +1608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1568,7 +1622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1579,7 +1633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1590,7 +1644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1601,7 +1655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1623,7 +1677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1645,7 +1699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1656,7 +1710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1667,7 +1721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1678,7 +1732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1692,7 +1746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1703,7 +1757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1717,7 +1771,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1728,7 +1782,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -1739,7 +1793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -1750,7 +1804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1761,7 +1815,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +1826,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -1783,7 +1837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
@@ -1794,7 +1848,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +1859,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1816,7 +1870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1827,7 +1881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1838,7 +1892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1849,7 +1903,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -1871,7 +1925,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
@@ -1882,7 +1936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>1</v>
       </c>
@@ -1893,12 +1947,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1920,7 +1974,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1931,7 +1985,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -1942,7 +1996,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1953,7 +2007,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>1</v>
       </c>
@@ -1964,7 +2018,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
@@ -1982,20 +2036,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="4"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2009,7 +2063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2023,7 +2077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2032,7 +2086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2046,7 +2100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2111,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2068,7 +2122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -2079,7 +2133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -2090,7 +2144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2101,7 +2155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2112,7 +2166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -2134,7 +2188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2145,7 +2199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -2170,7 +2224,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -2181,7 +2235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -2192,7 +2246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -2203,7 +2257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -2214,7 +2268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -2225,7 +2279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -2236,7 +2290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -2247,7 +2301,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2312,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
@@ -2269,7 +2323,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -2280,7 +2334,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -2291,7 +2345,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2367,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -2324,7 +2378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -2335,7 +2389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -2346,7 +2400,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>1</v>
       </c>
@@ -2364,20 +2418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="4"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2405,7 +2459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2413,7 +2467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2427,7 +2481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2438,7 +2492,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2449,7 +2503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -2460,7 +2514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -2471,7 +2525,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2482,7 +2536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2493,7 +2547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -2504,7 +2558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -2515,7 +2569,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2526,7 +2580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -2537,7 +2591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -2548,7 +2602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -2559,7 +2613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -2570,7 +2624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -2581,7 +2635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -2592,7 +2646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -2603,7 +2657,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
@@ -2614,7 +2668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -2625,7 +2679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -2636,7 +2690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -2647,7 +2701,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -2658,7 +2712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -2669,7 +2723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -2680,7 +2734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -2691,7 +2745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
@@ -2702,7 +2756,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -2713,7 +2767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
@@ -2724,7 +2778,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>1</v>
       </c>
@@ -2742,20 +2796,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="4"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2769,7 +2823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2783,7 +2837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2791,7 +2845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2805,7 +2859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2813,7 +2867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2824,7 +2878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -2835,7 +2889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -2846,7 +2900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2857,7 +2911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2868,7 +2922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -2879,7 +2933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -2890,7 +2944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2901,7 +2955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -2912,7 +2966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -2923,7 +2977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -2934,7 +2988,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -2945,7 +2999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -2956,7 +3010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -2967,7 +3021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -2978,7 +3032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
@@ -2989,7 +3043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -3000,7 +3054,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -3011,7 +3065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
@@ -3022,7 +3076,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -3033,7 +3087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
@@ -3044,7 +3098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
fix the startup code to work on ARM target
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3B289F42-43B4-42AD-8BB5-B1026DECDE9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E1102536-3867-468F-AC76-8C2BD48AD011}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20180611" sheetId="8" r:id="rId1"/>
-    <sheet name="20180122" sheetId="7" r:id="rId2"/>
-    <sheet name="20180120" sheetId="6" r:id="rId3"/>
-    <sheet name="20171011" sheetId="5" r:id="rId4"/>
-    <sheet name="20160602" sheetId="4" r:id="rId5"/>
-    <sheet name="20160601" sheetId="1" r:id="rId6"/>
+    <sheet name="20180803" sheetId="9" r:id="rId1"/>
+    <sheet name="20180611" sheetId="8" r:id="rId2"/>
+    <sheet name="20180122" sheetId="7" r:id="rId3"/>
+    <sheet name="20180120" sheetId="6" r:id="rId4"/>
+    <sheet name="20171011" sheetId="5" r:id="rId5"/>
+    <sheet name="20160602" sheetId="4" r:id="rId6"/>
+    <sheet name="20160601" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="60">
   <si>
     <t>State</t>
   </si>
@@ -615,11 +616,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="A31:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,6 +1077,467 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -1555,7 +2017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -2035,7 +2497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -2417,7 +2879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -2795,7 +3257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
first step for LLD rework
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E1102536-3867-468F-AC76-8C2BD48AD011}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E650E9CF-6B6F-4F1A-937B-C2458F236E15}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20180803" sheetId="9" r:id="rId1"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId1"/>
     <sheet name="20180611" sheetId="8" r:id="rId2"/>
     <sheet name="20180122" sheetId="7" r:id="rId3"/>
     <sheet name="20180120" sheetId="6" r:id="rId4"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="61">
   <si>
     <t>State</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>on_hold</t>
+  </si>
+  <si>
+    <t>os_start_init_mc is doing only peripheral now, the basic mcu init is done in os_exception_reset.s</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +826,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
@@ -834,7 +837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
@@ -845,7 +848,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -856,7 +859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -867,7 +870,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -878,7 +881,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -889,18 +892,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -911,7 +917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -922,7 +928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -933,7 +939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -944,7 +950,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -955,7 +961,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -966,7 +972,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -977,7 +983,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>59</v>
       </c>
@@ -988,7 +994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>48</v>
       </c>
@@ -1060,10 +1066,10 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C39" t="s">

</xml_diff>

<commit_message>
updated code block docu in folder input/pm,
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,27 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8199B14-0335-4240-A046-1E2ACB488FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C36C8C-8A88-45EB-BE53-31388E1712C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20180916" sheetId="11" r:id="rId1"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId2"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId3"/>
-    <sheet name="20180611" sheetId="8" r:id="rId4"/>
-    <sheet name="20180122" sheetId="7" r:id="rId5"/>
-    <sheet name="20180120" sheetId="6" r:id="rId6"/>
-    <sheet name="20171011" sheetId="5" r:id="rId7"/>
-    <sheet name="20160602" sheetId="4" r:id="rId8"/>
-    <sheet name="20160601" sheetId="1" r:id="rId9"/>
+    <sheet name="20180917" sheetId="12" r:id="rId1"/>
+    <sheet name="20180916" sheetId="11" r:id="rId2"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId3"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId4"/>
+    <sheet name="20180611" sheetId="8" r:id="rId5"/>
+    <sheet name="20180122" sheetId="7" r:id="rId6"/>
+    <sheet name="20180120" sheetId="6" r:id="rId7"/>
+    <sheet name="20171011" sheetId="5" r:id="rId8"/>
+    <sheet name="20160602" sheetId="4" r:id="rId9"/>
+    <sheet name="20160601" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="66">
   <si>
     <t>State</t>
   </si>
@@ -218,6 +219,10 @@
   </si>
   <si>
     <t>Traceability von Anforderungen zu Implementierung / Test</t>
+  </si>
+  <si>
+    <t>Debug for both targets not yet possible (e.g. gdb on x86 and Segger ICD for Cortex M4)
+https://www.mikrocontroller.net/topic/265600</t>
   </si>
 </sst>
 </file>
@@ -287,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -296,6 +301,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -633,11 +641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,15 +729,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,6 +1140,326 @@
       </c>
       <c r="C43" t="s">
         <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1141,6 +1469,514 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -1648,7 +2484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -2112,7 +2948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -2573,7 +3409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -3053,7 +3889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -3533,7 +4369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -3915,7 +4751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -4291,324 +5127,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updates for component test
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C36C8C-8A88-45EB-BE53-31388E1712C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541DA616-CB26-4A12-92A8-8EE3FA09043D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20180917" sheetId="12" r:id="rId1"/>
-    <sheet name="20180916" sheetId="11" r:id="rId2"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId3"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId4"/>
-    <sheet name="20180611" sheetId="8" r:id="rId5"/>
-    <sheet name="20180122" sheetId="7" r:id="rId6"/>
-    <sheet name="20180120" sheetId="6" r:id="rId7"/>
-    <sheet name="20171011" sheetId="5" r:id="rId8"/>
-    <sheet name="20160602" sheetId="4" r:id="rId9"/>
-    <sheet name="20160601" sheetId="1" r:id="rId10"/>
+    <sheet name="20181017" sheetId="13" r:id="rId1"/>
+    <sheet name="20180917" sheetId="12" r:id="rId2"/>
+    <sheet name="20180916" sheetId="11" r:id="rId3"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId4"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId5"/>
+    <sheet name="20180611" sheetId="8" r:id="rId6"/>
+    <sheet name="20180122" sheetId="7" r:id="rId7"/>
+    <sheet name="20180120" sheetId="6" r:id="rId8"/>
+    <sheet name="20171011" sheetId="5" r:id="rId9"/>
+    <sheet name="20160602" sheetId="4" r:id="rId10"/>
+    <sheet name="20160601" sheetId="1" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="66">
   <si>
     <t>State</t>
   </si>
@@ -641,11 +642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,6 +1150,384 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -1469,6 +1848,514 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -1976,7 +2863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2484,7 +3371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -2948,7 +3835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -3409,7 +4296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -3889,7 +4776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -4369,7 +5256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -4749,382 +5636,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix compile / assembler errors
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,29 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EAFBE2-724C-4296-A00F-F824BDC3BC88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46E32C0-480C-4EBB-9CE9-051B99B3976A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20181017" sheetId="13" r:id="rId1"/>
-    <sheet name="20180917" sheetId="12" r:id="rId2"/>
-    <sheet name="20180916" sheetId="11" r:id="rId3"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId4"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId5"/>
-    <sheet name="20180611" sheetId="8" r:id="rId6"/>
-    <sheet name="20180122" sheetId="7" r:id="rId7"/>
-    <sheet name="20180120" sheetId="6" r:id="rId8"/>
-    <sheet name="20171011" sheetId="5" r:id="rId9"/>
-    <sheet name="20160602" sheetId="4" r:id="rId10"/>
-    <sheet name="20160601" sheetId="1" r:id="rId11"/>
+    <sheet name="20181219" sheetId="14" r:id="rId1"/>
+    <sheet name="20181017" sheetId="13" r:id="rId2"/>
+    <sheet name="20180917" sheetId="12" r:id="rId3"/>
+    <sheet name="20180916" sheetId="11" r:id="rId4"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId5"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId6"/>
+    <sheet name="20180611" sheetId="8" r:id="rId7"/>
+    <sheet name="20180122" sheetId="7" r:id="rId8"/>
+    <sheet name="20180120" sheetId="6" r:id="rId9"/>
+    <sheet name="20171011" sheetId="5" r:id="rId10"/>
+    <sheet name="20160602" sheetId="4" r:id="rId11"/>
+    <sheet name="20160601" sheetId="1" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="67">
   <si>
     <t>State</t>
   </si>
@@ -224,6 +225,9 @@
   <si>
     <t>Debug for both targets not yet possible (e.g. gdb on x86 and Segger ICD for Cortex M4)
 https://www.mikrocontroller.net/topic/265600</t>
+  </si>
+  <si>
+    <t>see en.DM00046982.pdf page 192, not implemented in STM32F4 discovery board.</t>
   </si>
 </sst>
 </file>
@@ -644,11 +648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,17 +817,17 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,8 +840,8 @@
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
-        <v>58</v>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1061,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1068,7 +1072,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1079,18 +1083,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1101,7 +1108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1119,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>1</v>
       </c>
@@ -1123,7 +1130,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>1</v>
       </c>
@@ -1134,7 +1141,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
@@ -1152,6 +1159,388 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -1529,7 +1918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -1850,6 +2239,517 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B40" sqref="A40:B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2357,7 +3257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2865,7 +3765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3373,7 +4273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -3837,7 +4737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -4298,7 +5198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -4778,7 +5678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -5256,386 +6156,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
remove support for RTE and Diagnostic (both not yet implemented) to reach running OS faster...
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,30 +3,65 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46E32C0-480C-4EBB-9CE9-051B99B3976A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305DF03D-78B2-49EC-994A-1EA71CE76F81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20181219" sheetId="14" r:id="rId1"/>
-    <sheet name="20181017" sheetId="13" r:id="rId2"/>
-    <sheet name="20180917" sheetId="12" r:id="rId3"/>
-    <sheet name="20180916" sheetId="11" r:id="rId4"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId5"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId6"/>
-    <sheet name="20180611" sheetId="8" r:id="rId7"/>
-    <sheet name="20180122" sheetId="7" r:id="rId8"/>
-    <sheet name="20180120" sheetId="6" r:id="rId9"/>
-    <sheet name="20171011" sheetId="5" r:id="rId10"/>
-    <sheet name="20160602" sheetId="4" r:id="rId11"/>
-    <sheet name="20160601" sheetId="1" r:id="rId12"/>
+    <sheet name="20181230" sheetId="15" r:id="rId1"/>
+    <sheet name="20181219" sheetId="14" r:id="rId2"/>
+    <sheet name="20181017" sheetId="13" r:id="rId3"/>
+    <sheet name="20180917" sheetId="12" r:id="rId4"/>
+    <sheet name="20180916" sheetId="11" r:id="rId5"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId6"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId7"/>
+    <sheet name="20180611" sheetId="8" r:id="rId8"/>
+    <sheet name="20180122" sheetId="7" r:id="rId9"/>
+    <sheet name="20180120" sheetId="6" r:id="rId10"/>
+    <sheet name="20171011" sheetId="5" r:id="rId11"/>
+    <sheet name="20160602" sheetId="4" r:id="rId12"/>
+    <sheet name="20160601" sheetId="1" r:id="rId13"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{03ED17D8-BC1E-4306-81B2-67BC69C34E05}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="68">
   <si>
     <t>State</t>
   </si>
@@ -229,12 +264,15 @@
   <si>
     <t>see en.DM00046982.pdf page 192, not implemented in STM32F4 discovery board.</t>
   </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +295,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -297,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -311,6 +376,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -648,11 +716,494 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,26 +1287,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,18 +1317,18 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,7 +1339,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,10 +1347,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -807,13 +1358,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -821,13 +1369,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,66 +1382,69 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -904,57 +1452,54 @@
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,8 +1509,8 @@
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C26" t="s">
-        <v>32</v>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -975,8 +1520,8 @@
       <c r="B27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C27" t="s">
-        <v>33</v>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,7 +1532,7 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,158 +1543,133 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -1540,7 +2060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -1918,7 +2438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -2239,6 +2759,517 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2749,7 +3780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3257,7 +4288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3765,7 +4796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -4273,7 +5304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -4737,7 +5768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -5198,7 +6229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -5676,484 +6707,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
correct exception handling, update stack support
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -1,33 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EE5F02-4D9E-4153-B6CF-D45F1DE556CA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB88E5D-20DA-40B0-9114-ABC0D4336310}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2070" yWindow="375" windowWidth="15120" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24495" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190118" sheetId="16" r:id="rId1"/>
-    <sheet name="20181230" sheetId="15" r:id="rId2"/>
-    <sheet name="20181219" sheetId="14" r:id="rId3"/>
-    <sheet name="20181017" sheetId="13" r:id="rId4"/>
-    <sheet name="20180917" sheetId="12" r:id="rId5"/>
-    <sheet name="20180916" sheetId="11" r:id="rId6"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId7"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId8"/>
-    <sheet name="20180611" sheetId="8" r:id="rId9"/>
-    <sheet name="20180122" sheetId="7" r:id="rId10"/>
-    <sheet name="20180120" sheetId="6" r:id="rId11"/>
-    <sheet name="20171011" sheetId="5" r:id="rId12"/>
-    <sheet name="20160602" sheetId="4" r:id="rId13"/>
-    <sheet name="20160601" sheetId="1" r:id="rId14"/>
+    <sheet name="20190118 (2)" sheetId="17" r:id="rId1"/>
+    <sheet name="20190118" sheetId="16" r:id="rId2"/>
+    <sheet name="20181230" sheetId="15" r:id="rId3"/>
+    <sheet name="20181219" sheetId="14" r:id="rId4"/>
+    <sheet name="20181017" sheetId="13" r:id="rId5"/>
+    <sheet name="20180917" sheetId="12" r:id="rId6"/>
+    <sheet name="20180916" sheetId="11" r:id="rId7"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId8"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId9"/>
+    <sheet name="20180611" sheetId="8" r:id="rId10"/>
+    <sheet name="20180122" sheetId="7" r:id="rId11"/>
+    <sheet name="20180120" sheetId="6" r:id="rId12"/>
+    <sheet name="20171011" sheetId="5" r:id="rId13"/>
+    <sheet name="20160602" sheetId="4" r:id="rId14"/>
+    <sheet name="20160601" sheetId="1" r:id="rId15"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{1FFDBDF5-87C7-4A30-9AE8-665BA9130167}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -61,7 +96,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -96,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="70">
   <si>
     <t>State</t>
   </si>
@@ -403,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -420,6 +455,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -757,11 +793,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,10 +1046,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1240,6 +1276,467 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -1719,7 +2216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -2199,7 +2696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -2581,7 +3078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -2959,7 +3456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -3280,6 +3777,489 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="A21:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -3762,7 +4742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -4273,7 +5253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -4784,7 +5764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -5292,7 +6272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -5800,7 +6780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -6308,7 +7288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -6770,465 +7750,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix relevant static code analysis issues
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,32 +3,116 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B0DFFC-5806-45CA-B564-516EA8F7CA21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E492F79-CC9A-4110-9AE4-DC078E0D2B88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24495" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="24495" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190612" sheetId="17" r:id="rId1"/>
-    <sheet name="20190118" sheetId="16" r:id="rId2"/>
-    <sheet name="20181230" sheetId="15" r:id="rId3"/>
-    <sheet name="20181219" sheetId="14" r:id="rId4"/>
-    <sheet name="20181017" sheetId="13" r:id="rId5"/>
-    <sheet name="20180917" sheetId="12" r:id="rId6"/>
-    <sheet name="20180916" sheetId="11" r:id="rId7"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId8"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId9"/>
-    <sheet name="20180611" sheetId="8" r:id="rId10"/>
-    <sheet name="20180122" sheetId="7" r:id="rId11"/>
-    <sheet name="20180120" sheetId="6" r:id="rId12"/>
-    <sheet name="20171011" sheetId="5" r:id="rId13"/>
-    <sheet name="20160602" sheetId="4" r:id="rId14"/>
-    <sheet name="20160601" sheetId="1" r:id="rId15"/>
+    <sheet name="20190618" sheetId="18" r:id="rId1"/>
+    <sheet name="20190612" sheetId="17" r:id="rId2"/>
+    <sheet name="20190118" sheetId="16" r:id="rId3"/>
+    <sheet name="20181230" sheetId="15" r:id="rId4"/>
+    <sheet name="20181219" sheetId="14" r:id="rId5"/>
+    <sheet name="20181017" sheetId="13" r:id="rId6"/>
+    <sheet name="20180917" sheetId="12" r:id="rId7"/>
+    <sheet name="20180916" sheetId="11" r:id="rId8"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId9"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId10"/>
+    <sheet name="20180611" sheetId="8" r:id="rId11"/>
+    <sheet name="20180122" sheetId="7" r:id="rId12"/>
+    <sheet name="20180120" sheetId="6" r:id="rId13"/>
+    <sheet name="20171011" sheetId="5" r:id="rId14"/>
+    <sheet name="20160602" sheetId="4" r:id="rId15"/>
+    <sheet name="20160601" sheetId="1" r:id="rId16"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{E412CE63-7374-4C8A-9BC5-CABF042DF5C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{E1270DE5-6C24-4150-ACD9-D7D5F178E4BD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{22935517-9E2F-46EF-9B5E-9A87E9719D50}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -62,7 +146,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -96,7 +180,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -131,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="70">
   <si>
     <t>State</t>
   </si>
@@ -348,7 +432,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +482,19 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -793,11 +890,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,10 +1060,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1225,10 +1322,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C37" t="s">
@@ -1276,6 +1373,470 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -1736,7 +2297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -2216,7 +2777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -2696,7 +3257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -3078,7 +3639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -3456,7 +4017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -3777,6 +4338,489 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -4259,7 +5303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -4742,7 +5786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -5253,7 +6297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -5764,7 +6808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -6272,7 +7316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -6780,7 +7824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -7286,468 +8330,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
-  <dimension ref="A1:D39"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updates for rq and component test
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,33 +3,117 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E492F79-CC9A-4110-9AE4-DC078E0D2B88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3713B010-0279-4110-952C-E333DE2EC00A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="0" windowWidth="24495" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190618" sheetId="18" r:id="rId1"/>
-    <sheet name="20190612" sheetId="17" r:id="rId2"/>
-    <sheet name="20190118" sheetId="16" r:id="rId3"/>
-    <sheet name="20181230" sheetId="15" r:id="rId4"/>
-    <sheet name="20181219" sheetId="14" r:id="rId5"/>
-    <sheet name="20181017" sheetId="13" r:id="rId6"/>
-    <sheet name="20180917" sheetId="12" r:id="rId7"/>
-    <sheet name="20180916" sheetId="11" r:id="rId8"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId9"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId10"/>
-    <sheet name="20180611" sheetId="8" r:id="rId11"/>
-    <sheet name="20180122" sheetId="7" r:id="rId12"/>
-    <sheet name="20180120" sheetId="6" r:id="rId13"/>
-    <sheet name="20171011" sheetId="5" r:id="rId14"/>
-    <sheet name="20160602" sheetId="4" r:id="rId15"/>
-    <sheet name="20160601" sheetId="1" r:id="rId16"/>
+    <sheet name="20190619" sheetId="19" r:id="rId1"/>
+    <sheet name="20190618" sheetId="18" r:id="rId2"/>
+    <sheet name="20190612" sheetId="17" r:id="rId3"/>
+    <sheet name="20190118" sheetId="16" r:id="rId4"/>
+    <sheet name="20181230" sheetId="15" r:id="rId5"/>
+    <sheet name="20181219" sheetId="14" r:id="rId6"/>
+    <sheet name="20181017" sheetId="13" r:id="rId7"/>
+    <sheet name="20180917" sheetId="12" r:id="rId8"/>
+    <sheet name="20180916" sheetId="11" r:id="rId9"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId10"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId11"/>
+    <sheet name="20180611" sheetId="8" r:id="rId12"/>
+    <sheet name="20180122" sheetId="7" r:id="rId13"/>
+    <sheet name="20180120" sheetId="6" r:id="rId14"/>
+    <sheet name="20171011" sheetId="5" r:id="rId15"/>
+    <sheet name="20160602" sheetId="4" r:id="rId16"/>
+    <sheet name="20160601" sheetId="1" r:id="rId17"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{8B8F10F9-DF1A-44C2-9DB6-4F11A6A59C2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{1E655765-AC56-4713-8EE7-764D14567576}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{A4475986-7FEC-4295-9A02-090E7BBAD258}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -112,7 +196,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -146,7 +230,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -180,7 +264,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -215,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="71">
   <si>
     <t>State</t>
   </si>
@@ -427,6 +511,9 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>Anforderungsdokument schreiben (Anforderungen sollen die öffentlichen Schnittstellen auf C-Ebene entahlten, um direkt testbar zu sein)(welche c/h Dateien (inkl. Testdateien) gehören zu welcher Komponente,… Komponentenliste als Ergänzung der RQ schreiben)</t>
+  </si>
 </sst>
 </file>
 
@@ -535,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -553,6 +640,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -890,11 +989,505 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
-  <dimension ref="A1:E40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154B09E-5325-4DD5-92E9-AF8F7AC0400F}">
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,22 +1496,21 @@
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -932,7 +1524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -943,7 +1535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -957,7 +1549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -968,7 +1560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -979,18 +1571,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1001,7 +1593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1012,7 +1604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1059,21 +1651,21 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1083,11 +1675,11 @@
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -1098,281 +1690,307 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="6" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -1836,7 +2454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -2297,7 +2915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -2777,7 +3395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -3257,7 +3875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -3639,7 +4257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -4017,7 +4635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -4338,6 +4956,489 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -4820,7 +5921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -5303,7 +6404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -5786,7 +6887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -6297,7 +7398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -6808,7 +7909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -7316,7 +8417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -7822,512 +8923,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
-  <dimension ref="A1:D43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
implement stack cookie feature
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,35 +3,119 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F87B9F-3051-4087-8E9B-CA85587D22FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B83F61-F142-4ECA-AEA5-75457E9B43CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12345" yWindow="1965" windowWidth="24495" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190621" sheetId="20" r:id="rId1"/>
-    <sheet name="20190619" sheetId="19" r:id="rId2"/>
-    <sheet name="20190618" sheetId="18" r:id="rId3"/>
-    <sheet name="20190612" sheetId="17" r:id="rId4"/>
-    <sheet name="20190118" sheetId="16" r:id="rId5"/>
-    <sheet name="20181230" sheetId="15" r:id="rId6"/>
-    <sheet name="20181219" sheetId="14" r:id="rId7"/>
-    <sheet name="20181017" sheetId="13" r:id="rId8"/>
-    <sheet name="20180917" sheetId="12" r:id="rId9"/>
-    <sheet name="20180916" sheetId="11" r:id="rId10"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId11"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId12"/>
-    <sheet name="20180611" sheetId="8" r:id="rId13"/>
-    <sheet name="20180122" sheetId="7" r:id="rId14"/>
-    <sheet name="20180120" sheetId="6" r:id="rId15"/>
-    <sheet name="20171011" sheetId="5" r:id="rId16"/>
-    <sheet name="20160602" sheetId="4" r:id="rId17"/>
-    <sheet name="20160601" sheetId="1" r:id="rId18"/>
+    <sheet name="20190624" sheetId="21" r:id="rId1"/>
+    <sheet name="20190621" sheetId="20" r:id="rId2"/>
+    <sheet name="20190619" sheetId="19" r:id="rId3"/>
+    <sheet name="20190618" sheetId="18" r:id="rId4"/>
+    <sheet name="20190612" sheetId="17" r:id="rId5"/>
+    <sheet name="20190118" sheetId="16" r:id="rId6"/>
+    <sheet name="20181230" sheetId="15" r:id="rId7"/>
+    <sheet name="20181219" sheetId="14" r:id="rId8"/>
+    <sheet name="20181017" sheetId="13" r:id="rId9"/>
+    <sheet name="20180917" sheetId="12" r:id="rId10"/>
+    <sheet name="20180916" sheetId="11" r:id="rId11"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId12"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId13"/>
+    <sheet name="20180611" sheetId="8" r:id="rId14"/>
+    <sheet name="20180122" sheetId="7" r:id="rId15"/>
+    <sheet name="20180120" sheetId="6" r:id="rId16"/>
+    <sheet name="20171011" sheetId="5" r:id="rId17"/>
+    <sheet name="20160602" sheetId="4" r:id="rId18"/>
+    <sheet name="20160601" sheetId="1" r:id="rId19"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{638F588B-A3F5-4D49-9C97-23CFD62A2D1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{7B465065-9549-4FF5-B5DC-C98C2DFB83D6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{1B92272E-71BB-4496-80AB-ACE31730E79D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -114,7 +198,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -197,7 +281,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -280,7 +364,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -314,7 +398,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -348,7 +432,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -383,7 +467,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="72">
   <si>
     <t>State</t>
   </si>
@@ -1081,11 +1165,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C5AEEA-383D-43F6-9335-B41026418E17}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD6C500-6A83-41F0-839A-186C06EF142F}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,6 +1670,514 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2093,7 +2685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2601,7 +3193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -3065,7 +3657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -3526,7 +4118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -4006,7 +4598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -4486,7 +5078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -4868,7 +5460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -5246,7 +5838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -5567,6 +6159,511 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C5AEEA-383D-43F6-9335-B41026418E17}">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154B09E-5325-4DD5-92E9-AF8F7AC0400F}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -6060,7 +7157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -6543,7 +7640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -7026,7 +8123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -7509,7 +8606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -7992,7 +9089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -8503,7 +9600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -9012,512 +10109,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
-  <dimension ref="A1:D43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Mark the used functions in the requirements.xlsx with the color green, the white color function do not seem to be used.
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -1,38 +1,122 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBE839B-6C80-4E32-8684-7ED07B9AB8A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D6A845-1493-4619-8586-7A192C9CDD57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="600" windowWidth="24465" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190624" sheetId="21" r:id="rId1"/>
-    <sheet name="20190621" sheetId="20" r:id="rId2"/>
-    <sheet name="20190619" sheetId="19" r:id="rId3"/>
-    <sheet name="20190618" sheetId="18" r:id="rId4"/>
-    <sheet name="20190612" sheetId="17" r:id="rId5"/>
-    <sheet name="20190118" sheetId="16" r:id="rId6"/>
-    <sheet name="20181230" sheetId="15" r:id="rId7"/>
-    <sheet name="20181219" sheetId="14" r:id="rId8"/>
-    <sheet name="20181017" sheetId="13" r:id="rId9"/>
-    <sheet name="20180917" sheetId="12" r:id="rId10"/>
-    <sheet name="20180916" sheetId="11" r:id="rId11"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId12"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId13"/>
-    <sheet name="20180611" sheetId="8" r:id="rId14"/>
-    <sheet name="20180122" sheetId="7" r:id="rId15"/>
-    <sheet name="20180120" sheetId="6" r:id="rId16"/>
-    <sheet name="20171011" sheetId="5" r:id="rId17"/>
-    <sheet name="20160602" sheetId="4" r:id="rId18"/>
-    <sheet name="20160601" sheetId="1" r:id="rId19"/>
+    <sheet name="20190703" sheetId="22" r:id="rId1"/>
+    <sheet name="20190624" sheetId="21" r:id="rId2"/>
+    <sheet name="20190621" sheetId="20" r:id="rId3"/>
+    <sheet name="20190619" sheetId="19" r:id="rId4"/>
+    <sheet name="20190618" sheetId="18" r:id="rId5"/>
+    <sheet name="20190612" sheetId="17" r:id="rId6"/>
+    <sheet name="20190118" sheetId="16" r:id="rId7"/>
+    <sheet name="20181230" sheetId="15" r:id="rId8"/>
+    <sheet name="20181219" sheetId="14" r:id="rId9"/>
+    <sheet name="20181017" sheetId="13" r:id="rId10"/>
+    <sheet name="20180917" sheetId="12" r:id="rId11"/>
+    <sheet name="20180916" sheetId="11" r:id="rId12"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId13"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId14"/>
+    <sheet name="20180611" sheetId="8" r:id="rId15"/>
+    <sheet name="20180122" sheetId="7" r:id="rId16"/>
+    <sheet name="20180120" sheetId="6" r:id="rId17"/>
+    <sheet name="20171011" sheetId="5" r:id="rId18"/>
+    <sheet name="20160602" sheetId="4" r:id="rId19"/>
+    <sheet name="20160601" sheetId="1" r:id="rId20"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{6D5D2530-4F2D-4DE5-A954-1582EFE5C97E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{74674D28-1CB4-49D3-A9C5-E2932465D1C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{D48E33B5-8B80-4A5E-BFC6-CAED7B068275}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -115,7 +199,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -198,7 +282,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -281,7 +365,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -364,7 +448,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -398,7 +482,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -432,7 +516,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -467,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2489" uniqueCount="73">
   <si>
     <t>State</t>
   </si>
@@ -1168,11 +1252,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD6C500-6A83-41F0-839A-186C06EF142F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFA779-0BF0-49A7-871A-04F46D8C5308}">
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,6 +1768,517 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B40" sqref="A40:B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2191,7 +2786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2699,7 +3294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3207,7 +3802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -3671,7 +4266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -4132,7 +4727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -4612,7 +5207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -5092,7 +5687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -5474,7 +6069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -5852,7 +6447,523 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD6C500-6A83-41F0-839A-186C06EF142F}">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -6172,7 +7283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C5AEEA-383D-43F6-9335-B41026418E17}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -6677,7 +7788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154B09E-5325-4DD5-92E9-AF8F7AC0400F}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -7171,7 +8282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -7654,7 +8765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -8137,7 +9248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -8620,7 +9731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -9103,7 +10214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -9612,515 +10723,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
-  <dimension ref="A1:D43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B40" sqref="A40:B40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updates for time system
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,37 +3,239 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D6A845-1493-4619-8586-7A192C9CDD57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F88D315-6A45-4A23-89F3-9D966474194D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="600" windowWidth="24465" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190703" sheetId="22" r:id="rId1"/>
-    <sheet name="20190624" sheetId="21" r:id="rId2"/>
-    <sheet name="20190621" sheetId="20" r:id="rId3"/>
-    <sheet name="20190619" sheetId="19" r:id="rId4"/>
-    <sheet name="20190618" sheetId="18" r:id="rId5"/>
-    <sheet name="20190612" sheetId="17" r:id="rId6"/>
-    <sheet name="20190118" sheetId="16" r:id="rId7"/>
-    <sheet name="20181230" sheetId="15" r:id="rId8"/>
-    <sheet name="20181219" sheetId="14" r:id="rId9"/>
-    <sheet name="20181017" sheetId="13" r:id="rId10"/>
-    <sheet name="20180917" sheetId="12" r:id="rId11"/>
-    <sheet name="20180916" sheetId="11" r:id="rId12"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId13"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId14"/>
-    <sheet name="20180611" sheetId="8" r:id="rId15"/>
-    <sheet name="20180122" sheetId="7" r:id="rId16"/>
-    <sheet name="20180120" sheetId="6" r:id="rId17"/>
-    <sheet name="20171011" sheetId="5" r:id="rId18"/>
-    <sheet name="20160602" sheetId="4" r:id="rId19"/>
-    <sheet name="20160601" sheetId="1" r:id="rId20"/>
+    <sheet name="20190709" sheetId="24" r:id="rId1"/>
+    <sheet name="20190706" sheetId="23" r:id="rId2"/>
+    <sheet name="20190703" sheetId="22" r:id="rId3"/>
+    <sheet name="20190624" sheetId="21" r:id="rId4"/>
+    <sheet name="20190621" sheetId="20" r:id="rId5"/>
+    <sheet name="20190619" sheetId="19" r:id="rId6"/>
+    <sheet name="20190618" sheetId="18" r:id="rId7"/>
+    <sheet name="20190612" sheetId="17" r:id="rId8"/>
+    <sheet name="20190118" sheetId="16" r:id="rId9"/>
+    <sheet name="20181230" sheetId="15" r:id="rId10"/>
+    <sheet name="20181219" sheetId="14" r:id="rId11"/>
+    <sheet name="20181017" sheetId="13" r:id="rId12"/>
+    <sheet name="20180917" sheetId="12" r:id="rId13"/>
+    <sheet name="20180916" sheetId="11" r:id="rId14"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId15"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId16"/>
+    <sheet name="20180611" sheetId="8" r:id="rId17"/>
+    <sheet name="20180122" sheetId="7" r:id="rId18"/>
+    <sheet name="20180120" sheetId="6" r:id="rId19"/>
+    <sheet name="20171011" sheetId="5" r:id="rId20"/>
+    <sheet name="20160602" sheetId="4" r:id="rId21"/>
+    <sheet name="20160601" sheetId="1" r:id="rId22"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{3F09B7CB-3993-4DB4-A841-61287187EF52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{EF5411BD-4DED-4F66-B89F-531A64A73185}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{9B345440-AFA9-4DC4-9DDD-E5EBBDED34D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{03ED17D8-BC1E-4306-81B2-67BC69C34E05}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{CB9C43BE-FE1E-4935-A852-D079B0BF1EF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{ECA21A7F-EFC2-407D-9100-342E5067D7A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{FD185174-2276-42E7-B4E2-9A702FE63EBC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -116,7 +318,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -199,7 +401,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -282,7 +484,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -365,7 +567,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -448,7 +650,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -482,7 +684,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -516,42 +718,8 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{03ED17D8-BC1E-4306-81B2-67BC69C34E05}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Flash is done via ST-Link</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2489" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="77">
   <si>
     <t>State</t>
   </si>
@@ -776,6 +944,18 @@
   </si>
   <si>
     <t>Stack cookie feature</t>
+  </si>
+  <si>
+    <t>Create component test infrastructure</t>
+  </si>
+  <si>
+    <t>Configure PLL (see os_start_init_mc)</t>
+  </si>
+  <si>
+    <t>OS_DetermineNextTaskActivation, OS_TaskDispatcher handling</t>
+  </si>
+  <si>
+    <t>Overflow handling Time</t>
   </si>
 </sst>
 </file>
@@ -1252,11 +1432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFA779-0BF0-49A7-871A-04F46D8C5308}">
-  <dimension ref="A1:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428BC253-BD6E-4958-8478-F2F816930D32}">
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>63</v>
@@ -1721,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>64</v>
@@ -1732,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>70</v>
@@ -1758,6 +1938,50 @@
       </c>
       <c r="C43" s="8" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1768,6 +1992,1000 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2278,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2786,7 +4004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3294,7 +4512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3802,7 +5020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -4266,7 +5484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -4727,7 +5945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -5207,7 +6425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -5687,7 +6905,534 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF7BFB8-0F26-4ED2-BB97-A4F1681C485A}">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -6069,7 +7814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -6447,7 +8192,843 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFA779-0BF0-49A7-871A-04F46D8C5308}">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD6C500-6A83-41F0-839A-186C06EF142F}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -6963,327 +9544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C5AEEA-383D-43F6-9335-B41026418E17}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -7788,7 +10049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154B09E-5325-4DD5-92E9-AF8F7AC0400F}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -8282,7 +10543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -8765,7 +11026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -9248,7 +11509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -9729,998 +11990,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
-  <dimension ref="A1:E40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
-  <dimension ref="A1:D43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add TODOs into the source, where ever something is missing, add central config file (os_config.h)
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -1,41 +1,193 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F88D315-6A45-4A23-89F3-9D966474194D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902E7271-2838-46CB-869A-F015B7202C2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13935" yWindow="0" windowWidth="14865" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20190709" sheetId="24" r:id="rId1"/>
-    <sheet name="20190706" sheetId="23" r:id="rId2"/>
-    <sheet name="20190703" sheetId="22" r:id="rId3"/>
-    <sheet name="20190624" sheetId="21" r:id="rId4"/>
-    <sheet name="20190621" sheetId="20" r:id="rId5"/>
-    <sheet name="20190619" sheetId="19" r:id="rId6"/>
-    <sheet name="20190618" sheetId="18" r:id="rId7"/>
-    <sheet name="20190612" sheetId="17" r:id="rId8"/>
-    <sheet name="20190118" sheetId="16" r:id="rId9"/>
-    <sheet name="20181230" sheetId="15" r:id="rId10"/>
-    <sheet name="20181219" sheetId="14" r:id="rId11"/>
-    <sheet name="20181017" sheetId="13" r:id="rId12"/>
-    <sheet name="20180917" sheetId="12" r:id="rId13"/>
-    <sheet name="20180916" sheetId="11" r:id="rId14"/>
-    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId15"/>
-    <sheet name="20180803_04" sheetId="9" r:id="rId16"/>
-    <sheet name="20180611" sheetId="8" r:id="rId17"/>
-    <sheet name="20180122" sheetId="7" r:id="rId18"/>
-    <sheet name="20180120" sheetId="6" r:id="rId19"/>
-    <sheet name="20171011" sheetId="5" r:id="rId20"/>
-    <sheet name="20160602" sheetId="4" r:id="rId21"/>
-    <sheet name="20160601" sheetId="1" r:id="rId22"/>
+    <sheet name="20190904" sheetId="25" r:id="rId1"/>
+    <sheet name="20190709" sheetId="24" r:id="rId2"/>
+    <sheet name="20190706" sheetId="23" r:id="rId3"/>
+    <sheet name="20190703" sheetId="22" r:id="rId4"/>
+    <sheet name="20190624" sheetId="21" r:id="rId5"/>
+    <sheet name="20190621" sheetId="20" r:id="rId6"/>
+    <sheet name="20190619" sheetId="19" r:id="rId7"/>
+    <sheet name="20190618" sheetId="18" r:id="rId8"/>
+    <sheet name="20190612" sheetId="17" r:id="rId9"/>
+    <sheet name="20190118" sheetId="16" r:id="rId10"/>
+    <sheet name="20181230" sheetId="15" r:id="rId11"/>
+    <sheet name="20181219" sheetId="14" r:id="rId12"/>
+    <sheet name="20181017" sheetId="13" r:id="rId13"/>
+    <sheet name="20180917" sheetId="12" r:id="rId14"/>
+    <sheet name="20180916" sheetId="11" r:id="rId15"/>
+    <sheet name="20180811_0915_0916" sheetId="10" r:id="rId16"/>
+    <sheet name="20180803_04" sheetId="9" r:id="rId17"/>
+    <sheet name="20180611" sheetId="8" r:id="rId18"/>
+    <sheet name="20180122" sheetId="7" r:id="rId19"/>
+    <sheet name="20180120" sheetId="6" r:id="rId20"/>
+    <sheet name="20171011" sheetId="5" r:id="rId21"/>
+    <sheet name="20160602" sheetId="4" r:id="rId22"/>
+    <sheet name="20160601" sheetId="1" r:id="rId23"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{A6A1E09D-8AF9-41AE-8E8F-1A3FC2BFC54D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic MPU config used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{B25D26CD-4AEE-4838-BB85-F5DF0DF3BCE0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{6C4F016A-5EF2-4040-AFFC-3622E1527E6A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+der M4 hat nur einen DWT Timer, daher kein seperater Support hier nötig
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{F7D1D2C1-4285-4A13-8509-FF50B0BE069D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{03ED17D8-BC1E-4306-81B2-67BC69C34E05}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Flash is done via ST-Link</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -118,41 +270,7 @@
 </comments>
 </file>
 
-<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{03ED17D8-BC1E-4306-81B2-67BC69C34E05}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Flash is done via ST-Link</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -235,7 +353,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -318,7 +436,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -401,7 +519,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -484,7 +602,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -567,7 +685,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -650,7 +768,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -684,42 +802,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{F7D1D2C1-4285-4A13-8509-FF50B0BE069D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Flash is done via ST-Link</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="83">
   <si>
     <t>State</t>
   </si>
@@ -956,6 +1040,24 @@
   </si>
   <si>
     <t>Overflow handling Time</t>
+  </si>
+  <si>
+    <t>Add for every file a description</t>
+  </si>
+  <si>
+    <t>Add for every extern declaration / function definition a description</t>
+  </si>
+  <si>
+    <t>Fix every TODO in source code</t>
+  </si>
+  <si>
+    <t>introduce naming convention for functions and variables (capital letter, ….)</t>
+  </si>
+  <si>
+    <t>Every RAM allocation shall be done in os_ram.c / os_ram_shared.c</t>
+  </si>
+  <si>
+    <t>Every number assignment to an unsigned variable shall be postfixed with "u"</t>
   </si>
 </sst>
 </file>
@@ -1432,10 +1534,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428BC253-BD6E-4958-8478-F2F816930D32}">
-  <dimension ref="A1:E47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19297BD4-0C67-4F42-B9C4-4B37E3470F75}">
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -1984,6 +2086,72 @@
         <v>76</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1992,6 +2160,489 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="A21:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C0852E-FF5F-488E-8ED3-77814F9D79C4}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -2474,7 +3125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174D3C-1B85-40CE-AF9C-FDC8B875F0DA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -2985,7 +3636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B0935-D930-4663-AC4D-F1BEC88C1F1A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3496,7 +4147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261509A6-5DCD-40AB-ACFC-2B1D9886053E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -4004,7 +4655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4173E87-74DD-435C-9852-C0842515DB2A}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -4512,7 +5163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E669A02-E269-4E82-9123-1C669F98A382}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -5020,7 +5671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA40845-00EE-4886-BE03-11E8C8ED8C2A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -5484,7 +6135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -5945,7 +6596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -6425,7 +7076,567 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428BC253-BD6E-4958-8478-F2F816930D32}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -6905,7 +8116,1087 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF7BFB8-0F26-4ED2-BB97-A4F1681C485A}">
   <dimension ref="A1:E44"/>
   <sheetViews>
@@ -7432,1087 +9723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFA779-0BF0-49A7-871A-04F46D8C5308}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -9028,7 +10239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD6C500-6A83-41F0-839A-186C06EF142F}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -9544,7 +10755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C5AEEA-383D-43F6-9335-B41026418E17}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -10049,7 +11260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154B09E-5325-4DD5-92E9-AF8F7AC0400F}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -10543,7 +11754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD9EE9-7973-4458-8D85-CBF01CA75806}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -11026,7 +12237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A57A5F-23AE-440C-A22F-E1C5E462900F}">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -11507,487 +12718,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C56B23-64CB-41CB-939A-8BC0D31B7450}">
-  <dimension ref="A1:E40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
move static to global
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904773C3-F029-476B-AC60-83EFB51ED0F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471D831B-1A3B-4026-A2D6-24517A9051C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1650" windowWidth="14865" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190905" sheetId="26" r:id="rId1"/>
@@ -887,7 +887,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3114" uniqueCount="85">
   <si>
     <t>State</t>
   </si>
@@ -1145,6 +1145,17 @@
   </si>
   <si>
     <t>Update to current cppcheck version 1.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move static variables to global (can be analyzed via readsize.bat)
+stack_pos
+stack_used
+TASK_0
+TASK_1
+TASK_2
+TASK_3
+call_nr
+</t>
   </si>
 </sst>
 </file>
@@ -1622,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0A13E2-36A3-41F8-92FE-6228B8FF6033}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,8 +2218,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>1</v>
+      <c r="A51" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>14</v>
@@ -2218,8 +2229,8 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>1</v>
+      <c r="A52" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>14</v>
@@ -2248,6 +2259,17 @@
       </c>
       <c r="C54" s="8" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some compile issues
</commit_message>
<xml_diff>
--- a/input/pm/open_features.xlsx
+++ b/input/pm/open_features.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BB897D-89E3-4DC1-BBD6-A4589654C993}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789D2363-DB0B-4DB2-8BC3-DA1643C709D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1650" windowWidth="14865" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190905" sheetId="26" r:id="rId1"/>
@@ -887,7 +887,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3426" uniqueCount="85">
   <si>
     <t>State</t>
   </si>
@@ -1635,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0A13E2-36A3-41F8-92FE-6228B8FF6033}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,8 +2240,8 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>1</v>
+      <c r="A53" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>14</v>

</xml_diff>